<commit_message>
version control updated map colours updated sources table
</commit_message>
<xml_diff>
--- a/Data/3-4_FeSources/FeSources.xlsx
+++ b/Data/3-4_FeSources/FeSources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-4_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{C5D9A18D-45FD-479B-8496-973F64667A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{532DE205-F901-41E6-A1A5-6967F84EC043}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{C5D9A18D-45FD-479B-8496-973F64667A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8004607A-82FE-4E14-A7CF-8BB8D746A44D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
@@ -225,10 +225,10 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/reports/lmp/la/contents.aspx'&gt;ONS&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.gov.uk/government/publications/designated-employer-representative-bodies/notice-of-designated-employer-representative-bodies'&gt;Employer representative bodies&lt;/a&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">List of links to published Local skills improvement plans. </t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.gov.uk/government/publications/designated-employer-representative-bodies/notice-of-designated-employer-representative-bodies'&gt;Department for Education (gov.uk)&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -867,7 +867,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,10 +957,10 @@
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
         <v>59</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Backlog ID 116 117 118 adding new resources to the Further resources tab
</commit_message>
<xml_diff>
--- a/Data/3-4_FeSources/FeSources.xlsx
+++ b/Data/3-4_FeSources/FeSources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-4_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{C5D9A18D-45FD-479B-8496-973F64667A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8004607A-82FE-4E14-A7CF-8BB8D746A44D}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{FCD64274-F6DB-482E-8B8A-ECDC214852D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6D09820-8DBE-4125-ADEF-280FC615BE0F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>Source</t>
   </si>
@@ -180,21 +180,6 @@
     <t>&lt;a href='https://www.gov.uk/government/publications/neet-and-participation-local-authority-figures'&gt;NEET and participation: local authority figures - GOV.UK (www.gov.uk)&lt;/a&gt;</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">ESS 2023 - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Coming Summer 2023</t>
-    </r>
-  </si>
-  <si>
     <t>Employer Skills Survey including hard-to-fill and skill-shortage vacancies, employer skills needed in next 12 months, and percent of employers providing training</t>
   </si>
   <si>
@@ -229,13 +214,46 @@
   </si>
   <si>
     <t>&lt;a href='https://www.gov.uk/government/publications/designated-employer-representative-bodies/notice-of-designated-employer-representative-bodies'&gt;Department for Education (gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/find-statistics/employer-skills-survey/2022'&gt;Department for Education (gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.gov.uk/government/publications/ai-analysis-of-local-skills-improvement-plans'&gt;Department for Education (gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>UFS AI analysis of local skills improvement plans</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.gov.uk/government/publications/the-impact-of-ai-on-uk-jobs-and-training'&gt;Department for Education (gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>UFS impact of AI on UK jobs and training</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-local-statistics.beta.ons.gov.uk/'&gt;ONS&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>ONS Explore local statistics</t>
+  </si>
+  <si>
+    <t>Find, compare and visualise a range statistics about places in the United Kingdom down to ward level</t>
+  </si>
+  <si>
+    <t>UFS dashboards and data</t>
+  </si>
+  <si>
+    <t>Data and research to help understand current and emerging skills gaps and the type of jobs people take after training.</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.gov.uk/government/collections/job-and-skills-data'&gt;DfE&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +305,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0B0C0C"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -387,6 +417,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -406,9 +440,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -446,7 +480,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -552,7 +586,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -694,7 +728,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -702,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C0F38-06FA-4C4D-8065-41AFD4764DD8}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,13 +850,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -830,13 +864,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -844,15 +878,43 @@
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" t="s">
-        <v>57</v>
-      </c>
       <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -864,10 +926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACE25F3-3BBD-4BFB-8DFC-B2B552BE112F}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,26 +1019,44 @@
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="6" t="s">
         <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
       </c>
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add reports into loading
</commit_message>
<xml_diff>
--- a/Data/3-4_FeSources/FeSources.xlsx
+++ b/Data/3-4_FeSources/FeSources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-4_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95DD2B3C-5CAC-43D4-AB03-3CFA2B7C1C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{95DD2B3C-5CAC-43D4-AB03-3CFA2B7C1C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2930B7F6-5721-422C-A149-C958080F7DDB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" firstSheet="2" activeTab="2" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Report</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>&lt;a href='https://www.beta.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/qualityworkcomponentandcompositetablesuk2018'&gt;Job quality indicator tables, UK - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Higeher Education destination</t>
   </si>
   <si>
     <t xml:space="preserve">The data shows what people did after finishing their degree, by ethnicity. It includes people who graduated 1, 3, 5, and 10 years ago (up to March 2020) and the median earnings of graduates in employment. </t>
@@ -247,17 +244,14 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/'&gt;Explore Education Statistics&lt;/a&gt;</t>
   </si>
   <si>
-    <t>ONS Vacancies by SOC</t>
-  </si>
-  <si>
-    <t>Coming soon</t>
+    <t>Higher Education destination</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,13 +286,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -388,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -405,9 +392,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -418,17 +402,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,7 +733,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -777,29 +761,29 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -813,7 +797,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -824,36 +808,36 @@
     <col min="4" max="4" width="62.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -864,18 +848,18 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -887,18 +871,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACE25F3-3BBD-4BFB-8DFC-B2B552BE112F}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.26953125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="255.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="63.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.26953125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -913,163 +897,154 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="12" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="13" t="s">
+    </row>
+    <row r="13" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="13" t="s">
+    </row>
+    <row r="14" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="6" t="s">
-        <v>66</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>